<commit_message>
Odo muutmine töötab, ajaloo sisestamine pooleli
</commit_message>
<xml_diff>
--- a/Materjalid/Vehstory andmebaas.xlsx
+++ b/Materjalid/Vehstory andmebaas.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karmo\Documents\GitHub\Vehstory\Materjalid\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0348292A-F177-44C5-A186-257F836DFFF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="87">
   <si>
     <t>Kasutaja</t>
   </si>
@@ -216,9 +222,6 @@
     <t>updateLog</t>
   </si>
   <si>
-    <t>updateServices</t>
-  </si>
-  <si>
     <t>Vaade</t>
   </si>
   <si>
@@ -240,9 +243,6 @@
     <t>deleteClientAndVehicles</t>
   </si>
   <si>
-    <t>getServices</t>
-  </si>
-  <si>
     <t>Services</t>
   </si>
   <si>
@@ -252,9 +252,6 @@
     <t>ServiceLog</t>
   </si>
   <si>
-    <t>getLog</t>
-  </si>
-  <si>
     <t>logOut</t>
   </si>
   <si>
@@ -280,13 +277,31 @@
   </si>
   <si>
     <t>Insert new</t>
+  </si>
+  <si>
+    <t>Tehtud</t>
+  </si>
+  <si>
+    <t>getVehicleSelectedServices</t>
+  </si>
+  <si>
+    <t>updateSelectedServices</t>
+  </si>
+  <si>
+    <t>getSelectedServices</t>
+  </si>
+  <si>
+    <t>getServiceList</t>
+  </si>
+  <si>
+    <t>getVehicleServisceLog</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,7 +375,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,12 +465,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -539,13 +548,13 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -555,10 +564,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -579,13 +588,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>182217</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>455543</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>157370</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -593,7 +602,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8A4630E3-59DB-43DC-BD04-D2311678FA42}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A4630E3-59DB-43DC-BD04-D2311678FA42}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -669,13 +678,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>836544</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>99391</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>704023</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>59121</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -683,7 +692,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53F0EFAA-9699-4EF0-80B9-15592EB3CCDE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53F0EFAA-9699-4EF0-80B9-15592EB3CCDE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1026,13 +1035,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>775423</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>157370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>786706</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>99391</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1040,7 +1049,7 @@
         <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A91274EC-3A8B-40BA-9D00-F0F31A4481A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A91274EC-3A8B-40BA-9D00-F0F31A4481A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1082,13 +1091,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>414130</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>132522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>289891</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1096,7 +1105,7 @@
         <xdr:cNvPr id="8" name="TextBox 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5FD16B11-AB7E-410A-8241-93834647248A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FD16B11-AB7E-410A-8241-93834647248A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1280,13 +1289,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>289891</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>174506</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>836544</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>120098</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1294,7 +1303,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{23A36CD8-B9EF-429A-88EC-B77F4B4643AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23A36CD8-B9EF-429A-88EC-B77F4B4643AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1336,13 +1345,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8283</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>16565</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>33131</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>57978</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1350,7 +1359,7 @@
         <xdr:cNvPr id="16" name="TextBox 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5055CB6C-8DD7-4244-B9E0-00AAD961DBCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5055CB6C-8DD7-4244-B9E0-00AAD961DBCD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1410,7 +1419,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>- getLog</a:t>
+            <a:t>- getVehicleServisceLog</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" u="none" baseline="0">
@@ -1509,13 +1518,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>480535</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>59121</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>786706</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>16565</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1523,7 +1532,7 @@
         <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E0BA65F2-7E1D-4F0E-9551-C80ADF3620D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0BA65F2-7E1D-4F0E-9551-C80ADF3620D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1565,13 +1574,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418272</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8283</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>37272</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1579,7 +1588,7 @@
         <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{813C20A7-E479-44AB-B041-FDDACFAEEF63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{813C20A7-E479-44AB-B041-FDDACFAEEF63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1621,13 +1630,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>182218</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>140804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>198783</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>124239</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1635,7 +1644,7 @@
         <xdr:cNvPr id="23" name="TextBox 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BE2662BD-2730-4F54-95A9-AB3DCC4958DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE2662BD-2730-4F54-95A9-AB3DCC4958DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1762,13 +1771,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>704023</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>132522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>182218</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>174506</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1776,7 +1785,7 @@
         <xdr:cNvPr id="29" name="Straight Arrow Connector 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8063FD0F-3249-4B42-830F-4B1D5127D19E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8063FD0F-3249-4B42-830F-4B1D5127D19E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1818,13 +1827,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>704023</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>124239</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>174506</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1832,7 +1841,7 @@
         <xdr:cNvPr id="34" name="Straight Arrow Connector 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4A4A5B7-12D6-4904-8C0F-C466DC9E090B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4A4A5B7-12D6-4904-8C0F-C466DC9E090B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1874,98 +1883,98 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:D5" totalsRowShown="0">
-  <autoFilter ref="A3:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:D5" totalsRowShown="0">
+  <autoFilter ref="A3:D5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Nimi"/>
-    <tableColumn id="3" name="e-mail"/>
-    <tableColumn id="4" name="aktiivne"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nimi"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="e-mail"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="aktiivne"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="F3:P5" totalsRowShown="0">
-  <autoFilter ref="F3:P5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="F3:P5" totalsRowShown="0">
+  <autoFilter ref="F3:P5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Kasutaja ID"/>
-    <tableColumn id="3" name="Reg. nr"/>
-    <tableColumn id="4" name="Odo"/>
-    <tableColumn id="5" name="Tüüp"/>
-    <tableColumn id="6" name="Tootja"/>
-    <tableColumn id="7" name="Mudel"/>
-    <tableColumn id="8" name="Aasta"/>
-    <tableColumn id="9" name="Kütus"/>
-    <tableColumn id="10" name="mootori võimsus, kW"/>
-    <tableColumn id="11" name="aktiivne"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Kasutaja ID"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reg. nr"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Odo"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Tüüp"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Tootja"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Mudel"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Aasta"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Kütus"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="mootori võimsus, kW"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="aktiivne"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A9:C11" totalsRowShown="0">
-  <autoFilter ref="A9:C11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A8:C10" totalsRowShown="0">
+  <autoFilter ref="A8:C10" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Nimetus"/>
-    <tableColumn id="3" name="Aktiivne"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Nimetus"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Aktiivne"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="E9:K11" totalsRowShown="0">
-  <autoFilter ref="E9:K11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="E8:K10" totalsRowShown="0">
+  <autoFilter ref="E8:K10" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Sõiduki Id"/>
-    <tableColumn id="3" name="Hoolduse Id"/>
-    <tableColumn id="4" name="Välba_ühik"/>
-    <tableColumn id="5" name="Välba_väärtus"/>
-    <tableColumn id="6" name="Märkus"/>
-    <tableColumn id="7" name="Aktiivne"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Sõiduki Id"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Hoolduse Id"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Välba_ühik"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Välba_väärtus"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Märkus"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Aktiivne"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A15:G17" totalsRowShown="0">
-  <autoFilter ref="A15:G17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table5" displayName="Table5" ref="A13:G15" totalsRowShown="0">
+  <autoFilter ref="A13:G15" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Log_kp"/>
-    <tableColumn id="3" name="Sõiduki_id"/>
-    <tableColumn id="4" name="Hoolduse_id"/>
-    <tableColumn id="5" name="Kuupäev" dataDxfId="1"/>
-    <tableColumn id="6" name="p_odo"/>
-    <tableColumn id="7" name="Märkus"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Log_kp"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Sõiduki_id"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Hoolduse_id"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Kuupäev" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="p_odo"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Märkus"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A66:J68" totalsRowShown="0">
-  <autoFilter ref="A66:J68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A58:J60" totalsRowShown="0">
+  <autoFilter ref="A58:J60" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Nimetus"/>
-    <tableColumn id="2" name="Ühik"/>
-    <tableColumn id="3" name="Väärtus"/>
-    <tableColumn id="4" name="Kp_e"/>
-    <tableColumn id="5" name="Km_e"/>
-    <tableColumn id="6" name="Kp_j"/>
-    <tableColumn id="7" name="Km_j"/>
-    <tableColumn id="8" name="Kp_t" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Nimetus"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Ühik"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Väärtus"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Kp_e"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Km_e"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Kp_j"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Km_j"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Kp_t" dataDxfId="0">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Km_t"/>
-    <tableColumn id="10" name="Märkus"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Km_t"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="Märkus"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2014,7 +2023,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2066,7 +2075,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2260,21 +2269,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -2289,9 +2298,9 @@
     <col min="14" max="14" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2309,7 +2318,7 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -2317,7 +2326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2364,7 +2373,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2381,7 +2390,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>2</v>
       </c>
@@ -2392,608 +2401,654 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="13" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="4" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
       <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12">
+        <v>43863</v>
+      </c>
+      <c r="F14">
+        <v>15000</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" s="12">
+        <v>43863</v>
+      </c>
+      <c r="F15">
+        <v>15000</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="F46" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H54" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" s="6"/>
+      <c r="G55" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I57" s="23"/>
+      <c r="J57" s="10"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B58" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" t="s">
+        <v>37</v>
+      </c>
+      <c r="G58" t="s">
+        <v>38</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J58" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59">
+        <v>15000</v>
+      </c>
+      <c r="H59" s="12">
+        <f t="shared" ref="H59:H60" ca="1" si="0">TODAY()</f>
+        <v>44162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>49</v>
+      </c>
+      <c r="H60" s="12">
+        <f t="shared" ca="1" si="0"/>
+        <v>44162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="23"/>
+      <c r="D66" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="13" t="s">
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>56</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72">
         <v>1</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10">
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>68</v>
+      </c>
+      <c r="B73" s="19"/>
+      <c r="C73" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10">
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="19"/>
+      <c r="C74" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="19"/>
+      <c r="C75" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C76" t="s">
+        <v>67</v>
+      </c>
+      <c r="D76">
         <v>1</v>
       </c>
-      <c r="F10">
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C77" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77">
         <v>1</v>
       </c>
-      <c r="G10">
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C78" t="s">
+        <v>67</v>
+      </c>
+      <c r="D78">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="13" t="s">
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" t="s">
+        <v>70</v>
+      </c>
+      <c r="D79">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16">
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" t="s">
+        <v>69</v>
+      </c>
+      <c r="D80">
         <v>1</v>
       </c>
-      <c r="C16">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81" t="s">
+        <v>67</v>
+      </c>
+      <c r="D81">
         <v>1</v>
       </c>
-      <c r="D16">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" t="s">
+        <v>69</v>
+      </c>
+      <c r="D82">
         <v>1</v>
       </c>
-      <c r="E16" s="12">
-        <v>43863</v>
-      </c>
-      <c r="F16">
-        <v>15000</v>
-      </c>
-      <c r="G16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17" s="12">
-        <v>43863</v>
-      </c>
-      <c r="F17">
-        <v>15000</v>
-      </c>
-      <c r="G17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C83" t="s">
+        <v>70</v>
+      </c>
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" t="s">
+        <v>70</v>
+      </c>
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="F48" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="15"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B53" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D53" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F53" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="G53" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H53" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="H62" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F63" s="6"/>
-      <c r="G63" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I63" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J63" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="9.75" customHeight="1"/>
-    <row r="65" spans="1:10">
-      <c r="A65" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C65" s="22"/>
-      <c r="D65" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E65" s="22"/>
-      <c r="F65" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G65" s="22"/>
-      <c r="H65" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="I65" s="22"/>
-      <c r="J65" s="10"/>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" t="s">
-        <v>14</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D66" t="s">
-        <v>35</v>
-      </c>
-      <c r="E66" t="s">
-        <v>36</v>
-      </c>
-      <c r="F66" t="s">
-        <v>37</v>
-      </c>
-      <c r="G66" t="s">
-        <v>38</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I66" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J66" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="A67" t="s">
-        <v>45</v>
-      </c>
-      <c r="B67" t="s">
-        <v>46</v>
-      </c>
-      <c r="C67">
-        <v>15000</v>
-      </c>
-      <c r="H67" s="12">
-        <f t="shared" ref="H67:H68" ca="1" si="0">TODAY()</f>
-        <v>44161</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" t="s">
-        <v>49</v>
-      </c>
-      <c r="H68" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>44161</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G73" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="7.5" customHeight="1"/>
-    <row r="75" spans="1:10">
-      <c r="A75" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B75" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C75" s="22"/>
-      <c r="D75" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E75" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" t="s">
-        <v>14</v>
-      </c>
-      <c r="B76" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13">
-      <c r="A83" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
-    </row>
-    <row r="84" spans="1:13">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="13"/>
-      <c r="L84" s="13"/>
-      <c r="M84" s="13"/>
-    </row>
-    <row r="85" spans="1:13">
-      <c r="A85" t="s">
-        <v>56</v>
-      </c>
-      <c r="C85" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13">
-      <c r="A86" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B86" s="20"/>
-      <c r="C86" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13">
-      <c r="A87" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B87" s="20"/>
-      <c r="C87" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13">
-      <c r="A88" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B88" s="20"/>
-      <c r="C88" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13">
-      <c r="A89" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C89" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13">
-      <c r="A90" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C90" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13">
-      <c r="A91" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C91" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13">
-      <c r="A92" t="s">
-        <v>62</v>
-      </c>
-      <c r="C92" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13">
-      <c r="A93" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C93" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13">
-      <c r="A94" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C94" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13">
-      <c r="A95" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C95" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13">
-      <c r="A96" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C96" t="s">
-        <v>73</v>
-      </c>
+      <c r="D85" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="B66:C66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Selected Sevice parandused Sonarlinti kohaselt
</commit_message>
<xml_diff>
--- a/Materjalid/Vehstory andmebaas.xlsx
+++ b/Materjalid/Vehstory andmebaas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karmo\Documents\GitHub\Vehstory\Materjalid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5949DA67-DCDB-4375-8491-E7EF9D5F72E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE3CB4A-DFD2-43B8-9FDC-E7DBB50AFF25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -555,10 +555,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2284,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2649,7 +2649,7 @@
       <c r="G48" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="24" t="s">
+      <c r="H48" s="23" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2745,22 +2745,22 @@
       <c r="A57" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B57" s="23" t="s">
+      <c r="B57" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23" t="s">
+      <c r="C57" s="24"/>
+      <c r="D57" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23" t="s">
+      <c r="E57" s="24"/>
+      <c r="F57" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G57" s="23"/>
-      <c r="H57" s="23" t="s">
+      <c r="G57" s="24"/>
+      <c r="H57" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I57" s="23"/>
+      <c r="I57" s="24"/>
       <c r="J57" s="10"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -2807,7 +2807,7 @@
       </c>
       <c r="H59" s="12">
         <f t="shared" ref="H59:H60" ca="1" si="0">TODAY()</f>
-        <v>44162</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -2816,7 +2816,7 @@
       </c>
       <c r="H60" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44162</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -2849,10 +2849,10 @@
       <c r="A66" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B66" s="23" t="s">
+      <c r="B66" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C66" s="23"/>
+      <c r="C66" s="24"/>
       <c r="D66" s="21" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Sisse logimine backis töötab. Frontile vaja edasi anda onjekt. tokenit ei ole veel sisse pandud
</commit_message>
<xml_diff>
--- a/Materjalid/Vehstory andmebaas.xlsx
+++ b/Materjalid/Vehstory andmebaas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karmo\Documents\GitHub\Vehstory\Materjalid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906339B6-CE63-47E3-B0C2-0DD2976D001C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0429794-414F-4240-80C0-C0F88F9F346A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -310,7 +310,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +378,15 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="186"/>
@@ -479,7 +488,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -541,6 +550,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -548,7 +583,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -575,9 +610,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -585,6 +617,15 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -618,13 +659,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>182217</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>455543</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>157370</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -708,13 +749,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>836544</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>99391</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>704023</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>59121</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1065,13 +1106,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>775423</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>157370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>786706</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>99391</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1121,13 +1162,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>414130</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>132522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>289891</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1319,13 +1360,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>289891</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>174506</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>836544</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>120098</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1375,13 +1416,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8283</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>16565</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>33131</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>57978</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1548,13 +1589,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>480535</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>59121</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>786706</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>16565</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1604,13 +1645,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418272</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8283</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>37272</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1660,13 +1701,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>182218</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>140804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>198783</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>124239</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1801,13 +1842,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>704023</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>132522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>182218</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>174506</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1857,13 +1898,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>704023</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>124239</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>174506</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1926,8 +1967,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="F3:P5" totalsRowShown="0">
-  <autoFilter ref="F3:P5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A8:K10" totalsRowShown="0">
+  <autoFilter ref="A8:K10" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Kasutaja ID"/>
@@ -1946,8 +1987,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A8:C10" totalsRowShown="0">
-  <autoFilter ref="A8:C10" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A13:C15" totalsRowShown="0">
+  <autoFilter ref="A13:C15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Nimetus"/>
@@ -1958,8 +1999,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="E8:K10" totalsRowShown="0">
-  <autoFilter ref="E8:K10" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="E13:K15" totalsRowShown="0">
+  <autoFilter ref="E13:K15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Sõiduki Id"/>
@@ -1974,8 +2015,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table5" displayName="Table5" ref="A13:H15" totalsRowShown="0">
-  <autoFilter ref="A13:H15" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table5" displayName="Table5" ref="A18:H20" totalsRowShown="0">
+  <autoFilter ref="A18:H20" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Log_kp"/>
@@ -1991,8 +2032,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A58:J60" totalsRowShown="0">
-  <autoFilter ref="A58:J60" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A63:J65" totalsRowShown="0">
+  <autoFilter ref="A63:J65" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Nimetus"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Ühik"/>
@@ -2308,10 +2349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P102"/>
+  <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,7 +2366,7 @@
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
     <col min="14" max="14" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2353,9 +2394,6 @@
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2370,39 +2408,6 @@
       <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2411,129 +2416,106 @@
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
       </c>
       <c r="K8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9">
-        <v>15000</v>
+      <c r="G9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
-        <v>49</v>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
+      <c r="A12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H13" t="s">
+      <c r="K13" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2541,524 +2523,538 @@
       <c r="A14">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14">
         <v>1</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>1</v>
       </c>
-      <c r="E14" s="12">
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="12">
         <v>43863</v>
       </c>
-      <c r="F14">
+      <c r="F19">
         <v>15000</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C20">
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="D20">
         <v>2</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E20" s="12">
         <v>43863</v>
       </c>
-      <c r="F15">
+      <c r="F20">
         <v>15000</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>3</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C23">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C28">
         <v>3</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D28" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>5</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="6"/>
-      <c r="F46" s="6" t="s">
+      <c r="D51" s="6"/>
+      <c r="F51" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H46" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="J46" s="6" t="s">
+      <c r="J51" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B53" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C53" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D53" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E53" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="F53" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G48" s="16" t="s">
+      <c r="G53" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="23" t="s">
+      <c r="H53" s="23" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15" t="s">
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="20" t="s">
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B56" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C56" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D56" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E56" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="F51" s="20" t="s">
+      <c r="F56" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="G51" s="20" t="s">
+      <c r="G56" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H51" s="20" t="s">
+      <c r="H56" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H54" s="9" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H59" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B60" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C60" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D60" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E60" t="s">
         <v>27</v>
       </c>
-      <c r="F55" s="6"/>
-      <c r="G55" s="9" t="s">
+      <c r="F60" s="6"/>
+      <c r="G60" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I55" s="9" t="s">
+      <c r="I60" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J60" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+    <row r="61" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B57" s="24" t="s">
+      <c r="B62" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24" t="s">
+      <c r="C62" s="31"/>
+      <c r="D62" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24" t="s">
+      <c r="E62" s="31"/>
+      <c r="F62" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24" t="s">
+      <c r="G62" s="31"/>
+      <c r="H62" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="I57" s="24"/>
-      <c r="J57" s="10"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="I62" s="33"/>
+      <c r="J62" s="10"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B63" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C63" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D63" t="s">
         <v>35</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E63" t="s">
         <v>36</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F63" t="s">
         <v>37</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G63" t="s">
         <v>38</v>
       </c>
-      <c r="H58" s="6" t="s">
+      <c r="H63" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I58" s="6" t="s">
+      <c r="I63" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J58" s="6" t="s">
+      <c r="J63" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>45</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B64" t="s">
         <v>46</v>
       </c>
-      <c r="C59">
+      <c r="C64">
         <v>15000</v>
       </c>
-      <c r="H59" s="12">
-        <f t="shared" ref="H59:H60" ca="1" si="0">TODAY()</f>
-        <v>44166</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="H64" s="12">
+        <f t="shared" ref="H64:H65" ca="1" si="0">TODAY()</f>
+        <v>44168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>49</v>
       </c>
-      <c r="H60" s="12">
+      <c r="H65" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44166</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+        <v>44168</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B69" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C69" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D64" s="11" t="s">
+      <c r="D69" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="F69" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G69" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
+    <row r="70" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B66" s="24" t="s">
+      <c r="B71" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C66" s="24"/>
-      <c r="D66" s="21" t="s">
+      <c r="C71" s="31"/>
+      <c r="D71" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="21" t="s">
+      <c r="E71" s="21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B72" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="18" t="s">
+      <c r="C72" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="25" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B76" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C71" s="28" t="s">
+      <c r="C76" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="D76" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="E76" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F71" s="29" t="s">
+      <c r="F76" s="28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="26">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="25">
         <v>1</v>
       </c>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14">
+      <c r="B77" s="14"/>
+      <c r="C77" s="14">
         <v>1</v>
       </c>
-      <c r="D72" s="30">
+      <c r="D77" s="29">
         <v>43863</v>
       </c>
-      <c r="E72" s="14">
+      <c r="E77" s="14">
         <v>15000</v>
       </c>
-      <c r="F72" s="14" t="s">
+      <c r="F77" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="27">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="26">
         <v>2</v>
       </c>
-      <c r="B73" s="15"/>
-      <c r="C73" s="15">
+      <c r="B78" s="15"/>
+      <c r="C78" s="15">
         <v>2</v>
       </c>
-      <c r="D73" s="31">
+      <c r="D78" s="30">
         <v>43863</v>
       </c>
-      <c r="E73" s="15">
+      <c r="E78" s="15">
         <v>15000</v>
       </c>
-      <c r="F73" s="15" t="s">
+      <c r="F78" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
         <v>62</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D93" t="s">
         <v>81</v>
       </c>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="13"/>
-      <c r="K88" s="13"/>
-      <c r="L88" s="13"/>
-      <c r="M88" s="13"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="13"/>
+      <c r="K93" s="13"/>
+      <c r="L93" s="13"/>
+      <c r="M93" s="13"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>56</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C94" t="s">
         <v>63</v>
-      </c>
-      <c r="D89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>68</v>
-      </c>
-      <c r="B90" s="19"/>
-      <c r="C90" t="s">
-        <v>67</v>
-      </c>
-      <c r="D90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>72</v>
-      </c>
-      <c r="B91" s="19"/>
-      <c r="C91" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>74</v>
-      </c>
-      <c r="B92" s="19"/>
-      <c r="C92" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C93" t="s">
-        <v>67</v>
-      </c>
-      <c r="D93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C94" t="s">
-        <v>67</v>
       </c>
       <c r="D94">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
-        <v>59</v>
-      </c>
+      <c r="A95" t="s">
+        <v>68</v>
+      </c>
+      <c r="B95" s="19"/>
       <c r="C95" t="s">
         <v>67</v>
       </c>
@@ -3068,29 +3064,25 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>82</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B96" s="19"/>
       <c r="C96" t="s">
-        <v>70</v>
-      </c>
-      <c r="D96">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>83</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B97" s="19"/>
       <c r="C97" t="s">
-        <v>69</v>
-      </c>
-      <c r="D97">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>84</v>
+      <c r="A98" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="C98" t="s">
         <v>67</v>
@@ -3101,49 +3093,104 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C99" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D99">
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="22" t="s">
-        <v>73</v>
+      <c r="A100" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="C100" t="s">
-        <v>70</v>
-      </c>
-      <c r="D100" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C101" t="s">
         <v>70</v>
       </c>
-      <c r="D101" s="1"/>
+      <c r="D101">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>83</v>
+      </c>
+      <c r="C102" t="s">
+        <v>69</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>84</v>
+      </c>
+      <c r="C103" t="s">
+        <v>67</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C104" t="s">
+        <v>69</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C105" t="s">
+        <v>70</v>
+      </c>
+      <c r="D105" s="1"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>61</v>
+      </c>
+      <c r="C106" t="s">
+        <v>70</v>
+      </c>
+      <c r="D106" s="1"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>86</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C107" t="s">
         <v>71</v>
       </c>
-      <c r="D102" s="1"/>
+      <c r="D107" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="B71:C71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>